<commit_message>
réglages secondaires en cours
</commit_message>
<xml_diff>
--- a/Projet_Matrice/Matrices/60.xlsx
+++ b/Projet_Matrice/Matrices/60.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="329">
   <si>
     <t>Acquis</t>
   </si>
@@ -92,10 +92,10 @@
     <t>Reporting / Visualisation</t>
   </si>
   <si>
-    <t xml:space="preserve">Nom/Prénom : Kim Ly TRAN-MEYER </t>
-  </si>
-  <si>
-    <t>Nom de poste :Développeuse BI</t>
+    <t>Nom/Prénom  : Test Test</t>
+  </si>
+  <si>
+    <t>Nom de poste : Développeuse BI</t>
   </si>
   <si>
     <t>Hard Skills / outils</t>
@@ -110,6 +110,12 @@
     <t>Visuel</t>
   </si>
   <si>
+    <t>Microsoft SQL Server Analysis Services (SSAS)</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server Integration Services (SSIS)</t>
+  </si>
+  <si>
     <t>MongoDB</t>
   </si>
   <si>
@@ -122,6 +128,15 @@
     <t>ODI</t>
   </si>
   <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>SQL Server</t>
+  </si>
+  <si>
     <t>sybase</t>
   </si>
   <si>
@@ -275,6 +290,12 @@
     <t>scala</t>
   </si>
   <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Anglais</t>
+  </si>
+  <si>
     <t>Agiles</t>
   </si>
   <si>
@@ -284,9 +305,15 @@
     <t>CRM</t>
   </si>
   <si>
+    <t>Méthodologie Agile</t>
+  </si>
+  <si>
     <t>Méthodologie PMP</t>
   </si>
   <si>
+    <t>Méthodologie Scrum</t>
+  </si>
+  <si>
     <t>Méthodologie Waterfall</t>
   </si>
   <si>
@@ -308,6 +335,9 @@
     <t>asana</t>
   </si>
   <si>
+    <t>Confluence</t>
+  </si>
+  <si>
     <t>Dell Boomi</t>
   </si>
   <si>
@@ -329,6 +359,9 @@
     <t>HP QC</t>
   </si>
   <si>
+    <t>IBM Cognos</t>
+  </si>
+  <si>
     <t>IBM Infosphere MDM</t>
   </si>
   <si>
@@ -341,6 +374,12 @@
     <t>IntelliJ IDEA</t>
   </si>
   <si>
+    <t>Jira</t>
+  </si>
+  <si>
+    <t>Microsoft Teams</t>
+  </si>
+  <si>
     <t>Microsoft Visio</t>
   </si>
   <si>
@@ -365,12 +404,18 @@
     <t>Slack</t>
   </si>
   <si>
+    <t>Talend</t>
+  </si>
+  <si>
     <t>Tomcat / Jboss</t>
   </si>
   <si>
     <t>Trello</t>
   </si>
   <si>
+    <t>Visual Studio</t>
+  </si>
+  <si>
     <t>Visual Studio Code</t>
   </si>
   <si>
@@ -380,6 +425,9 @@
     <t>Docker</t>
   </si>
   <si>
+    <t>GitHub / GitLab</t>
+  </si>
+  <si>
     <t>Jenkins</t>
   </si>
   <si>
@@ -419,54 +467,6 @@
     <t>Xray</t>
   </si>
   <si>
-    <t>Confluence</t>
-  </si>
-  <si>
-    <t>GitHub / GitLab</t>
-  </si>
-  <si>
-    <t>Microsoft SQL Server Analysis Services (SSAS)</t>
-  </si>
-  <si>
-    <t>SQL Server</t>
-  </si>
-  <si>
-    <t>Anglais</t>
-  </si>
-  <si>
-    <t>Méthodologie Agile</t>
-  </si>
-  <si>
-    <t>Méthodologie Scrum</t>
-  </si>
-  <si>
-    <t>IBM Cognos</t>
-  </si>
-  <si>
-    <t>Visual Studio</t>
-  </si>
-  <si>
-    <t>Microsoft SQL Server Integration Services (SSIS)</t>
-  </si>
-  <si>
-    <t>Oracle</t>
-  </si>
-  <si>
-    <t>PostgreSQL</t>
-  </si>
-  <si>
-    <t>Jira</t>
-  </si>
-  <si>
-    <t>SQL</t>
-  </si>
-  <si>
-    <t>Microsoft Teams</t>
-  </si>
-  <si>
-    <t>Talend</t>
-  </si>
-  <si>
     <t>nom</t>
   </si>
   <si>
@@ -876,9 +876,6 @@
   </si>
   <si>
     <t>Tech lead Java</t>
-  </si>
-  <si>
-    <t>Nom de poste : Développeuse BI</t>
   </si>
   <si>
     <t>Soft Skills</t>
@@ -1316,19 +1313,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1695,7 +1686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1703,8 +1694,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1712,118 +1703,109 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="12" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="11" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="13" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="12" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="13" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="14" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="15" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="13" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="12" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="13" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="14" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="15" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -2179,88 +2161,88 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="45" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="45" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="45" width="34.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="46" width="115.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="42" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="42" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="42" width="34.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="43" width="115.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
+        <v>313</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="57.75">
+      <c r="A2" s="34">
+        <f>("⭐")</f>
+      </c>
+      <c r="B2" s="35" t="s">
         <v>314</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="57.75">
-      <c r="A2" s="37">
-        <f>("⭐")</f>
-      </c>
-      <c r="B2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>315</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="D2" s="37" t="s">
         <v>316</v>
       </c>
-      <c r="D2" s="40" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="57.75">
+      <c r="A3" s="34">
+        <f>("⭐⭐")</f>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="57.75">
-      <c r="A3" s="37">
-        <f>("⭐⭐")</f>
-      </c>
-      <c r="B3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="D3" s="37" t="s">
         <v>319</v>
       </c>
-      <c r="D3" s="40" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="57.75">
+      <c r="A4" s="34">
+        <f>("⭐⭐⭐")</f>
+      </c>
+      <c r="B4" s="35" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="57.75">
-      <c r="A4" s="37">
-        <f>("⭐⭐⭐")</f>
-      </c>
-      <c r="B4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>321</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="D4" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="D4" s="40" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="57.75">
+      <c r="A5" s="34">
+        <f>("⭐⭐⭐⭐")</f>
+      </c>
+      <c r="B5" s="35" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="57.75">
-      <c r="A5" s="37">
-        <f>("⭐⭐⭐⭐")</f>
-      </c>
-      <c r="B5" s="38" t="s">
+      <c r="C5" s="36" t="s">
         <v>324</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="D5" s="37" t="s">
         <v>325</v>
       </c>
-      <c r="D5" s="40" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="57.75">
+      <c r="A6" s="38">
+        <f>("⭐⭐⭐⭐⭐")</f>
+      </c>
+      <c r="B6" s="39" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="57.75">
-      <c r="A6" s="41">
-        <f>("⭐⭐⭐⭐⭐")</f>
-      </c>
-      <c r="B6" s="42" t="s">
+      <c r="C6" s="40" t="s">
         <v>327</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="D6" s="41" t="s">
         <v>328</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -2282,104 +2264,104 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="32" width="64.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="30" width="64.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="33" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="4" width="25.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="22" t="s">
-        <v>307</v>
+      <c r="A1" s="21" t="s">
+        <v>306</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="23"/>
+      <c r="G1" s="1"/>
       <c r="H1" s="3"/>
       <c r="I1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="52.5" customFormat="1" s="24">
-      <c r="A2" s="25" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="52.5" customFormat="1" s="22">
+      <c r="A2" s="23" t="s">
+        <v>307</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="24"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="78" customFormat="1" s="22">
+      <c r="A3" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="26"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="78" customFormat="1" s="24">
-      <c r="A3" s="25" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="24"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="64.5">
+      <c r="A4" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="26"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="64.5">
-      <c r="A4" s="25" t="s">
+      <c r="B4" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27">
+        <v>1</v>
+      </c>
+      <c r="F4" s="28">
+        <f>REPT("⭐",E4)</f>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="27">
+        <v>4</v>
+      </c>
+      <c r="I4" s="28">
+        <f>REPT("⭐",H4)</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="52.5" customFormat="1" s="22">
+      <c r="A5" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29">
-        <v>1</v>
-      </c>
-      <c r="F4" s="30">
-        <f>REPT("⭐",E4)</f>
-      </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="29">
-        <v>4</v>
-      </c>
-      <c r="I4" s="30">
-        <f>REPT("⭐",H4)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="52.5" customFormat="1" s="24">
-      <c r="A5" s="25" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="24"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="52.5" customFormat="1" s="22">
+      <c r="A6" s="29" t="s">
         <v>312</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="26"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="52.5" customFormat="1" s="24">
-      <c r="A6" s="31" t="s">
-        <v>313</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="26"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2394,7 +2376,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C161"/>
+  <dimension ref="A1:B161"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -2402,937 +2384,775 @@
   <cols>
     <col min="1" max="1" style="4" width="50.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="22.5">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21.75">
       <c r="A3" s="1" t="s">
-        <v>282</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="24">
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="B5" s="17"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="24">
       <c r="A6" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="B6" s="19" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="22.5">
+      <c r="A7" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="20" t="s">
+      <c r="B7" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="22.5">
+      <c r="A8" s="19" t="s">
         <v>285</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="20" t="s">
+      <c r="B8" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="22.5">
+      <c r="A9" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="20" t="s">
+      <c r="B9" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="22.5">
+      <c r="A10" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="20" t="s">
+      <c r="B10" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="22.5">
+      <c r="A11" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B11" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="22.5">
+      <c r="A12" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="22.5">
+      <c r="A13" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="22.5">
+      <c r="A14" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="22.5">
+      <c r="A15" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="22.5">
+      <c r="A16" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="22.5">
+      <c r="A17" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="22.5">
+      <c r="A18" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="22.5">
+      <c r="A19" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="22.5">
+      <c r="A20" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="B20" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="22.5">
-      <c r="A17" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="22.5">
-      <c r="A18" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="22.5">
-      <c r="A19" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="21"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="22.5">
-      <c r="A20" s="20" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="22.5">
+      <c r="A21" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B21" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="22.5">
+      <c r="A22" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="22.5">
+      <c r="A23" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="22.5">
+      <c r="A24" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="22.5">
+      <c r="A25" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="22.5">
+      <c r="A26" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="22.5">
-      <c r="A21" s="20" t="s">
-        <v>299</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="22.5">
-      <c r="A22" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="22.5">
-      <c r="A23" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="22.5">
-      <c r="A24" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="22.5">
-      <c r="A25" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="22.5">
-      <c r="A26" s="20" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="22.5">
+      <c r="A27" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="22.5">
-      <c r="A27" s="20" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="22.5">
+      <c r="A28" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="22.5">
-      <c r="A28" s="20" t="s">
-        <v>306</v>
-      </c>
-      <c r="B28" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="22.5">
+      <c r="A29" s="19"/>
+      <c r="B29" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="22.5">
-      <c r="A29" s="20"/>
-      <c r="B29" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="22.5">
+      <c r="A30" s="19"/>
+      <c r="B30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="22.5">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="22.5">
+      <c r="A31" s="19"/>
+      <c r="B31" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="22.5">
-      <c r="A31" s="20"/>
-      <c r="B31" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="22.5">
+      <c r="A32" s="19"/>
+      <c r="B32" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="22.5">
-      <c r="A32" s="20"/>
-      <c r="B32" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="22.5">
+      <c r="A33" s="19"/>
+      <c r="B33" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="22.5">
-      <c r="A33" s="20"/>
-      <c r="B33" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="22.5">
+      <c r="A34" s="19"/>
+      <c r="B34" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="22.5">
-      <c r="A34" s="20"/>
-      <c r="B34" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="22.5">
+      <c r="A35" s="19"/>
+      <c r="B35" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="22.5">
-      <c r="A35" s="20"/>
-      <c r="B35" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="22.5">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="22.5">
-      <c r="A36" s="20"/>
-      <c r="B36" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="22.5">
+      <c r="A37" s="19"/>
+      <c r="B37" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="22.5">
-      <c r="A37" s="20"/>
-      <c r="B37" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="22.5">
+      <c r="A38" s="19"/>
+      <c r="B38" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="22.5">
-      <c r="A38" s="20"/>
-      <c r="B38" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="22.5">
+      <c r="A39" s="19"/>
+      <c r="B39" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="22.5">
-      <c r="A39" s="20"/>
-      <c r="B39" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="22.5">
+      <c r="A40" s="19"/>
+      <c r="B40" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="22.5">
-      <c r="A40" s="20"/>
-      <c r="B40" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="22.5">
+      <c r="A41" s="19"/>
+      <c r="B41" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="22.5">
-      <c r="A41" s="20"/>
-      <c r="B41" s="21" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="22.5">
+      <c r="A42" s="19"/>
+      <c r="B42" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="22.5">
-      <c r="A42" s="20"/>
-      <c r="B42" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="22.5">
       <c r="A43" s="1"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="1"/>
+      <c r="B43" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="22.5">
       <c r="A44" s="1"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="1"/>
+      <c r="B44" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="22.5">
       <c r="A45" s="1"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="1"/>
+      <c r="B45" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="22.5">
       <c r="A46" s="1"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="1"/>
+      <c r="B46" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="22.5">
       <c r="A47" s="1"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="1"/>
+      <c r="B47" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="22.5">
       <c r="A48" s="1"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="1"/>
+      <c r="B48" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="22.5">
       <c r="A49" s="1"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="1"/>
+      <c r="B49" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="22.5">
       <c r="A50" s="1"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="1"/>
+      <c r="B50" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="22.5">
       <c r="A51" s="1"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="1"/>
+      <c r="B51" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="22.5">
       <c r="A52" s="1"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="1"/>
+      <c r="B52" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="22.5">
       <c r="A53" s="1"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="1"/>
+      <c r="B53" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="22.5">
       <c r="A54" s="1"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="1"/>
+      <c r="B54" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="22.5">
       <c r="A55" s="1"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="1"/>
+      <c r="B55" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="22.5">
       <c r="A56" s="1"/>
-      <c r="B56" s="21"/>
-      <c r="C56" s="1"/>
+      <c r="B56" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="22.5">
       <c r="A57" s="1"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="1"/>
+      <c r="B57" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="22.5">
       <c r="A58" s="1"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="1"/>
+      <c r="B58" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="22.5">
       <c r="A59" s="1"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="1"/>
+      <c r="B59" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="22.5">
       <c r="A60" s="1"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="1"/>
+      <c r="B60" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="22.5">
       <c r="A61" s="1"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="1"/>
+      <c r="B61" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="22.5">
       <c r="A62" s="1"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="1"/>
+      <c r="B62" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="22.5">
       <c r="A63" s="1"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="1"/>
+      <c r="B63" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="22.5">
       <c r="A64" s="1"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="1"/>
+      <c r="B64" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="22.5">
       <c r="A65" s="1"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="1"/>
+      <c r="B65" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="22.5">
       <c r="A66" s="1"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="1"/>
+      <c r="B66" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="22.5">
       <c r="A67" s="1"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="1"/>
+      <c r="B67" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="22.5">
       <c r="A68" s="1"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="1"/>
+      <c r="B68" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="22.5">
       <c r="A69" s="1"/>
-      <c r="B69" s="21"/>
-      <c r="C69" s="1"/>
+      <c r="B69" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="22.5">
       <c r="A70" s="1"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="1"/>
+      <c r="B70" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="22.5">
       <c r="A71" s="1"/>
-      <c r="B71" s="21"/>
-      <c r="C71" s="1"/>
+      <c r="B71" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="22.5">
       <c r="A72" s="1"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="1"/>
+      <c r="B72" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="22.5">
       <c r="A73" s="1"/>
-      <c r="B73" s="21"/>
-      <c r="C73" s="1"/>
+      <c r="B73" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="22.5">
       <c r="A74" s="1"/>
-      <c r="B74" s="21"/>
-      <c r="C74" s="1"/>
+      <c r="B74" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="22.5">
       <c r="A75" s="1"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="1"/>
+      <c r="B75" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="22.5">
       <c r="A76" s="1"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="1"/>
+      <c r="B76" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="22.5">
       <c r="A77" s="1"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="1"/>
+      <c r="B77" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="22.5">
       <c r="A78" s="1"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="1"/>
+      <c r="B78" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="22.5">
       <c r="A79" s="1"/>
-      <c r="B79" s="21"/>
-      <c r="C79" s="1"/>
+      <c r="B79" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="22.5">
       <c r="A80" s="1"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="1"/>
+      <c r="B80" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="22.5">
       <c r="A81" s="1"/>
-      <c r="B81" s="21"/>
-      <c r="C81" s="1"/>
+      <c r="B81" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="22.5">
       <c r="A82" s="1"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="1"/>
+      <c r="B82" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="22.5">
       <c r="A83" s="1"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="1"/>
+      <c r="B83" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="22.5">
       <c r="A84" s="1"/>
-      <c r="B84" s="21"/>
-      <c r="C84" s="1"/>
+      <c r="B84" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="22.5">
       <c r="A85" s="1"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="1"/>
+      <c r="B85" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="22.5">
       <c r="A86" s="1"/>
-      <c r="B86" s="21"/>
-      <c r="C86" s="1"/>
+      <c r="B86" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="22.5">
       <c r="A87" s="1"/>
-      <c r="B87" s="21"/>
-      <c r="C87" s="1"/>
+      <c r="B87" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="22.5">
       <c r="A88" s="1"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="1"/>
+      <c r="B88" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="22.5">
       <c r="A89" s="1"/>
-      <c r="B89" s="21"/>
-      <c r="C89" s="1"/>
+      <c r="B89" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="22.5">
       <c r="A90" s="1"/>
-      <c r="B90" s="21"/>
-      <c r="C90" s="1"/>
+      <c r="B90" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="22.5">
       <c r="A91" s="1"/>
-      <c r="B91" s="21"/>
-      <c r="C91" s="1"/>
+      <c r="B91" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="22.5">
       <c r="A92" s="1"/>
-      <c r="B92" s="21"/>
-      <c r="C92" s="1"/>
+      <c r="B92" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="22.5">
       <c r="A93" s="1"/>
-      <c r="B93" s="21"/>
-      <c r="C93" s="1"/>
+      <c r="B93" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="22.5">
       <c r="A94" s="1"/>
-      <c r="B94" s="21"/>
-      <c r="C94" s="1"/>
+      <c r="B94" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="22.5">
       <c r="A95" s="1"/>
-      <c r="B95" s="21"/>
-      <c r="C95" s="1"/>
+      <c r="B95" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="22.5">
       <c r="A96" s="1"/>
-      <c r="B96" s="21"/>
-      <c r="C96" s="1"/>
+      <c r="B96" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="22.5">
       <c r="A97" s="1"/>
-      <c r="B97" s="21"/>
-      <c r="C97" s="1"/>
+      <c r="B97" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="22.5">
       <c r="A98" s="1"/>
-      <c r="B98" s="21"/>
-      <c r="C98" s="1"/>
+      <c r="B98" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="22.5">
       <c r="A99" s="1"/>
-      <c r="B99" s="21"/>
-      <c r="C99" s="1"/>
+      <c r="B99" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="22.5">
       <c r="A100" s="1"/>
-      <c r="B100" s="21"/>
-      <c r="C100" s="1"/>
+      <c r="B100" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="22.5">
       <c r="A101" s="1"/>
-      <c r="B101" s="21"/>
-      <c r="C101" s="1"/>
+      <c r="B101" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="22.5">
       <c r="A102" s="1"/>
-      <c r="B102" s="21"/>
-      <c r="C102" s="1"/>
+      <c r="B102" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="22.5">
       <c r="A103" s="1"/>
-      <c r="B103" s="21"/>
-      <c r="C103" s="1"/>
+      <c r="B103" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="22.5">
       <c r="A104" s="1"/>
-      <c r="B104" s="21"/>
-      <c r="C104" s="1"/>
+      <c r="B104" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="22.5">
       <c r="A105" s="1"/>
-      <c r="B105" s="21"/>
-      <c r="C105" s="1"/>
+      <c r="B105" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="22.5">
       <c r="A106" s="1"/>
-      <c r="B106" s="21"/>
-      <c r="C106" s="1"/>
+      <c r="B106" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="22.5">
       <c r="A107" s="1"/>
-      <c r="B107" s="21"/>
-      <c r="C107" s="1"/>
+      <c r="B107" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="22.5">
       <c r="A108" s="1"/>
-      <c r="B108" s="21"/>
-      <c r="C108" s="1"/>
+      <c r="B108" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="22.5">
       <c r="A109" s="1"/>
-      <c r="B109" s="21"/>
-      <c r="C109" s="1"/>
+      <c r="B109" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="22.5">
       <c r="A110" s="1"/>
-      <c r="B110" s="21"/>
-      <c r="C110" s="1"/>
+      <c r="B110" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="22.5">
       <c r="A111" s="1"/>
-      <c r="B111" s="21"/>
-      <c r="C111" s="1"/>
+      <c r="B111" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="22.5">
       <c r="A112" s="1"/>
-      <c r="B112" s="21"/>
-      <c r="C112" s="1"/>
+      <c r="B112" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="22.5">
       <c r="A113" s="1"/>
-      <c r="B113" s="21"/>
-      <c r="C113" s="1"/>
+      <c r="B113" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="22.5">
       <c r="A114" s="1"/>
-      <c r="B114" s="21"/>
-      <c r="C114" s="1"/>
+      <c r="B114" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="22.5">
       <c r="A115" s="1"/>
-      <c r="B115" s="21"/>
-      <c r="C115" s="1"/>
+      <c r="B115" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="22.5">
       <c r="A116" s="1"/>
-      <c r="B116" s="21"/>
-      <c r="C116" s="1"/>
+      <c r="B116" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="22.5">
       <c r="A117" s="1"/>
-      <c r="B117" s="21"/>
-      <c r="C117" s="1"/>
+      <c r="B117" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="22.5">
       <c r="A118" s="1"/>
-      <c r="B118" s="21"/>
-      <c r="C118" s="1"/>
+      <c r="B118" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="22.5">
       <c r="A119" s="1"/>
-      <c r="B119" s="21"/>
-      <c r="C119" s="1"/>
+      <c r="B119" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="22.5">
       <c r="A120" s="1"/>
-      <c r="B120" s="21"/>
-      <c r="C120" s="1"/>
+      <c r="B120" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="22.5">
       <c r="A121" s="1"/>
-      <c r="B121" s="21"/>
-      <c r="C121" s="1"/>
+      <c r="B121" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="22.5">
       <c r="A122" s="1"/>
-      <c r="B122" s="21"/>
-      <c r="C122" s="1"/>
+      <c r="B122" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="22.5">
       <c r="A123" s="1"/>
-      <c r="B123" s="21"/>
-      <c r="C123" s="1"/>
+      <c r="B123" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="22.5">
       <c r="A124" s="1"/>
-      <c r="B124" s="21"/>
-      <c r="C124" s="1"/>
+      <c r="B124" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="22.5">
       <c r="A125" s="1"/>
-      <c r="B125" s="21"/>
-      <c r="C125" s="1"/>
+      <c r="B125" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="22.5">
       <c r="A126" s="1"/>
-      <c r="B126" s="21"/>
-      <c r="C126" s="1"/>
+      <c r="B126" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="22.5">
       <c r="A127" s="1"/>
-      <c r="B127" s="21"/>
-      <c r="C127" s="1"/>
+      <c r="B127" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="22.5">
       <c r="A128" s="1"/>
-      <c r="B128" s="21"/>
-      <c r="C128" s="1"/>
+      <c r="B128" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="22.5">
       <c r="A129" s="1"/>
-      <c r="B129" s="21"/>
-      <c r="C129" s="1"/>
+      <c r="B129" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="22.5">
       <c r="A130" s="1"/>
-      <c r="B130" s="21"/>
-      <c r="C130" s="1"/>
+      <c r="B130" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="22.5">
       <c r="A131" s="1"/>
-      <c r="B131" s="21"/>
-      <c r="C131" s="1"/>
+      <c r="B131" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="22.5">
       <c r="A132" s="1"/>
-      <c r="B132" s="21"/>
-      <c r="C132" s="1"/>
+      <c r="B132" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="22.5">
       <c r="A133" s="1"/>
-      <c r="B133" s="21"/>
-      <c r="C133" s="1"/>
+      <c r="B133" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="22.5">
       <c r="A134" s="1"/>
-      <c r="B134" s="21"/>
-      <c r="C134" s="1"/>
+      <c r="B134" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="22.5">
       <c r="A135" s="1"/>
-      <c r="B135" s="21"/>
-      <c r="C135" s="1"/>
+      <c r="B135" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="22.5">
       <c r="A136" s="1"/>
-      <c r="B136" s="21"/>
-      <c r="C136" s="1"/>
+      <c r="B136" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="22.5">
       <c r="A137" s="1"/>
-      <c r="B137" s="21"/>
-      <c r="C137" s="1"/>
+      <c r="B137" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="22.5">
       <c r="A138" s="1"/>
-      <c r="B138" s="21"/>
-      <c r="C138" s="1"/>
+      <c r="B138" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="22.5">
       <c r="A139" s="1"/>
-      <c r="B139" s="21"/>
-      <c r="C139" s="1"/>
+      <c r="B139" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="22.5">
       <c r="A140" s="1"/>
-      <c r="B140" s="21"/>
-      <c r="C140" s="1"/>
+      <c r="B140" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="22.5">
       <c r="A141" s="1"/>
-      <c r="B141" s="21"/>
-      <c r="C141" s="1"/>
+      <c r="B141" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="22.5">
       <c r="A142" s="1"/>
-      <c r="B142" s="21"/>
-      <c r="C142" s="1"/>
+      <c r="B142" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="22.5">
       <c r="A143" s="1"/>
-      <c r="B143" s="21"/>
-      <c r="C143" s="1"/>
+      <c r="B143" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="22.5">
       <c r="A144" s="1"/>
-      <c r="B144" s="21"/>
-      <c r="C144" s="1"/>
+      <c r="B144" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="22.5">
       <c r="A145" s="1"/>
-      <c r="B145" s="21"/>
-      <c r="C145" s="1"/>
+      <c r="B145" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="22.5">
       <c r="A146" s="1"/>
-      <c r="B146" s="21"/>
-      <c r="C146" s="1"/>
+      <c r="B146" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="22.5">
       <c r="A147" s="1"/>
-      <c r="B147" s="21"/>
-      <c r="C147" s="1"/>
+      <c r="B147" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="22.5">
       <c r="A148" s="1"/>
-      <c r="B148" s="21"/>
-      <c r="C148" s="1"/>
+      <c r="B148" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="22.5">
       <c r="A149" s="1"/>
-      <c r="B149" s="21"/>
-      <c r="C149" s="1"/>
+      <c r="B149" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="22.5">
       <c r="A150" s="1"/>
-      <c r="B150" s="21"/>
-      <c r="C150" s="1"/>
+      <c r="B150" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="22.5">
       <c r="A151" s="1"/>
-      <c r="B151" s="21"/>
-      <c r="C151" s="1"/>
+      <c r="B151" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="22.5">
       <c r="A152" s="1"/>
-      <c r="B152" s="21"/>
-      <c r="C152" s="1"/>
+      <c r="B152" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="22.5">
       <c r="A153" s="1"/>
-      <c r="B153" s="21"/>
-      <c r="C153" s="1"/>
+      <c r="B153" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
-      <c r="C154" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
-      <c r="C155" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
-      <c r="C156" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
-      <c r="C157" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
-      <c r="C158" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
-      <c r="C159" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
-      <c r="C160" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
-      <c r="C161" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3356,11 +3176,11 @@
     <col min="1" max="1" style="4" width="2.862142857142857" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="30.14785714285714" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="4" width="38.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="27.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="27.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="5.576428571428571" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="4" width="4.719285714285714" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="4" width="47.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="15.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -3393,7 +3213,7 @@
       <c r="G2" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3402,7 +3222,7 @@
       <c r="B3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D3" s="1" t="s">
@@ -3422,7 +3242,7 @@
       <c r="B4" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D4" s="1" t="s">
@@ -3442,7 +3262,7 @@
       <c r="B5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D5" s="1" t="s">
@@ -3462,7 +3282,7 @@
       <c r="B6" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D6" s="1" t="s">
@@ -3482,7 +3302,7 @@
       <c r="B7" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D7" s="1" t="s">
@@ -3502,7 +3322,7 @@
       <c r="B8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D8" s="1" t="s">
@@ -3522,7 +3342,7 @@
       <c r="B9" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D9" s="1" t="s">
@@ -3542,7 +3362,7 @@
       <c r="B10" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D10" s="1" t="s">
@@ -3562,7 +3382,7 @@
       <c r="B11" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D11" s="1" t="s">
@@ -3582,7 +3402,7 @@
       <c r="B12" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D12" s="1" t="s">
@@ -3602,7 +3422,7 @@
       <c r="B13" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D13" s="1" t="s">
@@ -3622,7 +3442,7 @@
       <c r="B14" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D14" s="1" t="s">
@@ -3642,7 +3462,7 @@
       <c r="B15" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D15" s="1" t="s">
@@ -3662,7 +3482,7 @@
       <c r="B16" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D16" s="1" t="s">
@@ -3682,7 +3502,7 @@
       <c r="B17" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D17" s="1" t="s">
@@ -3702,7 +3522,7 @@
       <c r="B18" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D18" s="1" t="s">
@@ -3722,7 +3542,7 @@
       <c r="B19" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D19" s="1" t="s">
@@ -3742,7 +3562,7 @@
       <c r="B20" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D20" s="1" t="s">
@@ -3762,7 +3582,7 @@
       <c r="B21" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D21" s="1" t="s">
@@ -3782,7 +3602,7 @@
       <c r="B22" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D22" s="1" t="s">
@@ -3802,7 +3622,7 @@
       <c r="B23" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D23" s="1" t="s">
@@ -3822,7 +3642,7 @@
       <c r="B24" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D24" s="1" t="s">
@@ -3842,7 +3662,7 @@
       <c r="B25" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D25" s="1" t="s">
@@ -3862,7 +3682,7 @@
       <c r="B26" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D26" s="1" t="s">
@@ -3882,7 +3702,7 @@
       <c r="B27" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D27" s="1" t="s">
@@ -3902,7 +3722,7 @@
       <c r="B28" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D28" s="1" t="s">
@@ -3922,7 +3742,7 @@
       <c r="B29" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D29" s="1" t="s">
@@ -3942,7 +3762,7 @@
       <c r="B30" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D30" s="1" t="s">
@@ -3962,7 +3782,7 @@
       <c r="B31" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D31" s="1" t="s">
@@ -3982,7 +3802,7 @@
       <c r="B32" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D32" s="1" t="s">
@@ -4002,7 +3822,7 @@
       <c r="B33" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D33" s="1" t="s">
@@ -4022,7 +3842,7 @@
       <c r="B34" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D34" s="1" t="s">
@@ -4042,7 +3862,7 @@
       <c r="B35" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D35" s="1" t="s">
@@ -4062,7 +3882,7 @@
       <c r="B36" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D36" s="1" t="s">
@@ -4082,7 +3902,7 @@
       <c r="B37" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D37" s="1" t="s">
@@ -4102,7 +3922,7 @@
       <c r="B38" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D38" s="1" t="s">
@@ -4122,7 +3942,7 @@
       <c r="B39" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D39" s="1" t="s">
@@ -4135,10 +3955,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="1"/>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C40" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D40" s="1" t="s">
@@ -4154,7 +3974,7 @@
       <c r="B41" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C41" s="15">
+      <c r="C41" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D41" s="1" t="s">
@@ -4170,7 +3990,7 @@
       <c r="B42" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C42" s="15">
+      <c r="C42" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D42" s="1" t="s">
@@ -4186,7 +4006,7 @@
       <c r="B43" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C43" s="15">
+      <c r="C43" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D43" s="1" t="s">
@@ -4202,7 +4022,7 @@
       <c r="B44" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C44" s="15">
+      <c r="C44" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D44" s="1" t="s">
@@ -4215,10 +4035,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="1"/>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="C45" s="15">
+      <c r="C45" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D45" s="1" t="s">
@@ -4234,7 +4054,7 @@
       <c r="B46" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C46" s="15">
+      <c r="C46" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D46" s="1" t="s">
@@ -4250,7 +4070,7 @@
       <c r="B47" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C47" s="15">
+      <c r="C47" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D47" s="1" t="s">
@@ -4266,7 +4086,7 @@
       <c r="B48" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C48" s="15">
+      <c r="C48" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D48" s="1" t="s">
@@ -4282,7 +4102,7 @@
       <c r="B49" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C49" s="15">
+      <c r="C49" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D49" s="1" t="s">
@@ -4298,7 +4118,7 @@
       <c r="B50" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C50" s="15">
+      <c r="C50" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D50" s="1" t="s">
@@ -4314,7 +4134,7 @@
       <c r="B51" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C51" s="15">
+      <c r="C51" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D51" s="1" t="s">
@@ -4330,7 +4150,7 @@
       <c r="B52" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C52" s="15">
+      <c r="C52" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D52" s="1" t="s">
@@ -4346,7 +4166,7 @@
       <c r="B53" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C53" s="15">
+      <c r="C53" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D53" s="1" t="s">
@@ -4362,7 +4182,7 @@
       <c r="B54" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C54" s="15">
+      <c r="C54" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D54" s="1" t="s">
@@ -4378,7 +4198,7 @@
       <c r="B55" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C55" s="15">
+      <c r="C55" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D55" s="1" t="s">
@@ -4394,7 +4214,7 @@
       <c r="B56" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C56" s="15">
+      <c r="C56" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D56" s="1" t="s">
@@ -4410,7 +4230,7 @@
       <c r="B57" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C57" s="15">
+      <c r="C57" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D57" s="1" t="s">
@@ -4426,7 +4246,7 @@
       <c r="B58" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C58" s="15">
+      <c r="C58" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D58" s="1" t="s">
@@ -4442,7 +4262,7 @@
       <c r="B59" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C59" s="15">
+      <c r="C59" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D59" s="1" t="s">
@@ -4458,7 +4278,7 @@
       <c r="B60" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C60" s="15">
+      <c r="C60" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D60" s="1" t="s">
@@ -4474,7 +4294,7 @@
       <c r="B61" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C61" s="15">
+      <c r="C61" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D61" s="1" t="s">
@@ -4490,7 +4310,7 @@
       <c r="B62" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C62" s="15">
+      <c r="C62" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D62" s="1" t="s">
@@ -4506,7 +4326,7 @@
       <c r="B63" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C63" s="15">
+      <c r="C63" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D63" s="1" t="s">
@@ -4522,7 +4342,7 @@
       <c r="B64" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C64" s="15">
+      <c r="C64" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D64" s="1" t="s">
@@ -4535,10 +4355,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="1"/>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="C65" s="15">
+      <c r="C65" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D65" s="1" t="s">
@@ -4554,7 +4374,7 @@
       <c r="B66" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C66" s="15">
+      <c r="C66" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D66" s="1" t="s">
@@ -4570,7 +4390,7 @@
       <c r="B67" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C67" s="15">
+      <c r="C67" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D67" s="1" t="s">
@@ -4586,7 +4406,7 @@
       <c r="B68" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C68" s="15">
+      <c r="C68" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D68" s="1" t="s">
@@ -4602,7 +4422,7 @@
       <c r="B69" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C69" s="15">
+      <c r="C69" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D69" s="1" t="s">
@@ -4618,7 +4438,7 @@
       <c r="B70" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C70" s="15">
+      <c r="C70" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D70" s="1" t="s">
@@ -4634,7 +4454,7 @@
       <c r="B71" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C71" s="15">
+      <c r="C71" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D71" s="1" t="s">
@@ -4650,7 +4470,7 @@
       <c r="B72" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C72" s="15">
+      <c r="C72" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D72" s="1" t="s">
@@ -4666,7 +4486,7 @@
       <c r="B73" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C73" s="15">
+      <c r="C73" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D73" s="1" t="s">
@@ -4682,7 +4502,7 @@
       <c r="B74" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C74" s="15">
+      <c r="C74" s="14">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D74" s="1" t="s">
@@ -4712,19 +4532,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="51.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="51.57642857142857" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="44.29071428571429" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="16.290714285714284" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="4" width="27.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="15">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="3"/>
       <c r="D1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="22.5">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
@@ -4732,7 +4552,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -4752,7 +4572,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="22.5">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -4766,7 +4586,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -4774,13 +4594,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -4788,13 +4608,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D8" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -4808,7 +4628,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -4822,7 +4642,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -4836,7 +4656,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -4850,54 +4670,54 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="21">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9">
         <v>3</v>
       </c>
-      <c r="C13" s="9">
-        <v>0</v>
-      </c>
       <c r="D13" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="21">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9">
         <v>3</v>
       </c>
-      <c r="C14" s="9">
-        <v>0</v>
-      </c>
       <c r="D14" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="21">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" s="9">
         <v>0</v>
@@ -4906,12 +4726,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" s="9">
         <v>0</v>
@@ -4920,12 +4740,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="9">
         <v>0</v>
@@ -4934,12 +4754,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" s="9">
         <v>0</v>
@@ -4948,12 +4768,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="9">
         <v>0</v>
@@ -4962,12 +4782,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="9">
         <v>0</v>
@@ -4976,12 +4796,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="9">
         <v>0</v>
@@ -4990,7 +4810,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -5004,7 +4824,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -5018,7 +4838,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -5032,12 +4852,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="9">
         <v>0</v>
@@ -5046,12 +4866,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="9">
         <v>0</v>
@@ -5060,12 +4880,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="9">
         <v>0</v>
@@ -5074,12 +4894,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="9">
         <v>0</v>
@@ -5088,12 +4908,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="9">
         <v>0</v>
@@ -5102,7 +4922,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
@@ -5116,7 +4936,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1" t="s">
         <v>51</v>
       </c>
@@ -5130,7 +4950,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1" t="s">
         <v>52</v>
       </c>
@@ -5144,7 +4964,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1" t="s">
         <v>53</v>
       </c>
@@ -5158,7 +4978,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="1" t="s">
         <v>54</v>
       </c>
@@ -5172,7 +4992,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="1" t="s">
         <v>55</v>
       </c>
@@ -5186,7 +5006,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="1" t="s">
         <v>56</v>
       </c>
@@ -5200,7 +5020,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="1" t="s">
         <v>57</v>
       </c>
@@ -5214,7 +5034,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="1" t="s">
         <v>58</v>
       </c>
@@ -5228,7 +5048,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="1" t="s">
         <v>59</v>
       </c>
@@ -5242,7 +5062,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="1" t="s">
         <v>60</v>
       </c>
@@ -5256,7 +5076,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="1" t="s">
         <v>61</v>
       </c>
@@ -5270,7 +5090,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="1" t="s">
         <v>62</v>
       </c>
@@ -5284,7 +5104,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="1" t="s">
         <v>63</v>
       </c>
@@ -5298,12 +5118,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45" s="9">
         <v>0</v>
@@ -5312,12 +5132,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46" s="9">
         <v>0</v>
@@ -5326,12 +5146,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C47" s="9">
         <v>0</v>
@@ -5340,12 +5160,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C48" s="9">
         <v>0</v>
@@ -5354,12 +5174,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C49" s="9">
         <v>0</v>
@@ -5368,12 +5188,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50" s="9">
         <v>0</v>
@@ -5382,12 +5202,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" s="9">
         <v>0</v>
@@ -5396,12 +5216,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52" s="9">
         <v>0</v>
@@ -5410,12 +5230,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C53" s="9">
         <v>0</v>
@@ -5424,12 +5244,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C54" s="9">
         <v>0</v>
@@ -5438,12 +5258,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C55" s="9">
         <v>0</v>
@@ -5452,12 +5272,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56" s="9">
         <v>0</v>
@@ -5466,12 +5286,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C57" s="9">
         <v>0</v>
@@ -5480,7 +5300,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="1" t="s">
         <v>77</v>
       </c>
@@ -5494,7 +5314,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="1" t="s">
         <v>78</v>
       </c>
@@ -5508,7 +5328,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="1" t="s">
         <v>79</v>
       </c>
@@ -5522,7 +5342,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="1" t="s">
         <v>80</v>
       </c>
@@ -5536,12 +5356,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C62" s="9">
         <v>0</v>
@@ -5550,12 +5370,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C63" s="9">
         <v>0</v>
@@ -5564,12 +5384,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C64" s="9">
         <v>0</v>
@@ -5578,12 +5398,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C65" s="9">
         <v>0</v>
@@ -5592,12 +5412,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C66" s="9">
         <v>0</v>
@@ -5606,35 +5426,35 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C67" s="9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D67" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C68" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D68" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="1" t="s">
         <v>88</v>
       </c>
@@ -5648,7 +5468,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="1" t="s">
         <v>89</v>
       </c>
@@ -5662,12 +5482,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C71" s="9">
         <v>0</v>
@@ -5676,26 +5496,26 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C72" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D72" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C73" s="9">
         <v>0</v>
@@ -5704,26 +5524,26 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C74" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D74" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C75" s="9">
         <v>0</v>
@@ -5732,12 +5552,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C76" s="9">
         <v>0</v>
@@ -5746,12 +5566,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C77" s="9">
         <v>0</v>
@@ -5760,12 +5580,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C78" s="9">
         <v>0</v>
@@ -5774,12 +5594,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C79" s="9">
         <v>0</v>
@@ -5788,7 +5608,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="1" t="s">
         <v>99</v>
       </c>
@@ -5802,7 +5622,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="1" t="s">
         <v>100</v>
       </c>
@@ -5816,7 +5636,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="1" t="s">
         <v>101</v>
       </c>
@@ -5824,13 +5644,13 @@
         <v>11</v>
       </c>
       <c r="C82" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="1" t="s">
         <v>102</v>
       </c>
@@ -5844,7 +5664,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="1" t="s">
         <v>103</v>
       </c>
@@ -5858,7 +5678,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="1" t="s">
         <v>104</v>
       </c>
@@ -5872,7 +5692,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="1" t="s">
         <v>105</v>
       </c>
@@ -5886,7 +5706,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="1" t="s">
         <v>106</v>
       </c>
@@ -5900,7 +5720,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="1" t="s">
         <v>107</v>
       </c>
@@ -5914,7 +5734,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="1" t="s">
         <v>108</v>
       </c>
@@ -5928,7 +5748,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="1" t="s">
         <v>109</v>
       </c>
@@ -5936,13 +5756,13 @@
         <v>11</v>
       </c>
       <c r="C90" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D90" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="1" t="s">
         <v>110</v>
       </c>
@@ -5956,7 +5776,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="1" t="s">
         <v>111</v>
       </c>
@@ -5970,7 +5790,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="1" t="s">
         <v>112</v>
       </c>
@@ -5984,7 +5804,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="1" t="s">
         <v>113</v>
       </c>
@@ -5998,40 +5818,40 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C95" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D95" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C96" s="9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D96" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C97" s="9">
         <v>0</v>
@@ -6040,12 +5860,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C98" s="9">
         <v>0</v>
@@ -6054,12 +5874,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C99" s="9">
         <v>0</v>
@@ -6068,12 +5888,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C100" s="9">
         <v>0</v>
@@ -6082,12 +5902,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C101" s="9">
         <v>0</v>
@@ -6096,12 +5916,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C102" s="9">
         <v>0</v>
@@ -6110,12 +5930,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C103" s="9">
         <v>0</v>
@@ -6124,12 +5944,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C104" s="9">
         <v>0</v>
@@ -6138,26 +5958,26 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C105" s="9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D105" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
       <c r="A106" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C106" s="9">
         <v>0</v>
@@ -6166,12 +5986,12 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C107" s="9">
         <v>0</v>
@@ -6180,157 +6000,209 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
       <c r="A108" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C108" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D108" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109" s="9">
+        <v>0</v>
+      </c>
+      <c r="D109" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
+      <c r="A110" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110" s="9">
+        <v>0</v>
+      </c>
+      <c r="D110" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
+      <c r="A111" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C111" s="9">
+        <v>0</v>
+      </c>
+      <c r="D111" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
+      <c r="A112" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C112" s="9">
+        <v>1</v>
+      </c>
+      <c r="D112" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
+      <c r="A113" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C113" s="9">
+        <v>0</v>
+      </c>
+      <c r="D113" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
+      <c r="A114" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C114" s="9">
+        <v>0</v>
+      </c>
+      <c r="D114" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
+      <c r="A115" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C115" s="9">
+        <v>0</v>
+      </c>
+      <c r="D115" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
+      <c r="A116" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C116" s="9">
+        <v>0</v>
+      </c>
+      <c r="D116" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
+      <c r="A117" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C117" s="9">
+        <v>0</v>
+      </c>
+      <c r="D117" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
+      <c r="A118" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C118" s="9">
+        <v>0</v>
+      </c>
+      <c r="D118" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
+      <c r="A119" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C119" s="9">
+        <v>0</v>
+      </c>
+      <c r="D119" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
+      <c r="A120" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C120" s="9">
+        <v>0</v>
+      </c>
+      <c r="D120" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
+      <c r="A121" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C121" s="9">
+        <v>0</v>
+      </c>
+      <c r="D121" s="10">
+        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
+      <c r="A122" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C109" s="9">
-        <v>0</v>
-      </c>
-      <c r="D109" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75" hidden="1">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="9">
-        <v>0</v>
-      </c>
-      <c r="D110" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75" hidden="1">
-      <c r="A111" s="11"/>
-      <c r="B111" s="12"/>
-      <c r="C111" s="9">
-        <v>0</v>
-      </c>
-      <c r="D111" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75" hidden="1">
-      <c r="A112" s="12"/>
-      <c r="B112" s="12"/>
-      <c r="C112" s="9">
-        <v>0</v>
-      </c>
-      <c r="D112" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75" hidden="1">
-      <c r="A113" s="11"/>
-      <c r="B113" s="12"/>
-      <c r="C113" s="9">
-        <v>0</v>
-      </c>
-      <c r="D113" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75" hidden="1">
-      <c r="A114" s="11"/>
-      <c r="B114" s="12"/>
-      <c r="C114" s="9">
-        <v>0</v>
-      </c>
-      <c r="D114" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75" hidden="1">
-      <c r="A115" s="11"/>
-      <c r="B115" s="12"/>
-      <c r="C115" s="9">
-        <v>0</v>
-      </c>
-      <c r="D115" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75" hidden="1">
-      <c r="A116" s="11"/>
-      <c r="B116" s="12"/>
-      <c r="C116" s="9">
-        <v>0</v>
-      </c>
-      <c r="D116" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75" hidden="1">
-      <c r="A117" s="11"/>
-      <c r="B117" s="12"/>
-      <c r="C117" s="9">
-        <v>0</v>
-      </c>
-      <c r="D117" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75" hidden="1">
-      <c r="A118" s="13"/>
-      <c r="B118" s="12"/>
-      <c r="C118" s="9">
-        <v>0</v>
-      </c>
-      <c r="D118" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75" hidden="1">
-      <c r="A119" s="13"/>
-      <c r="B119" s="12"/>
-      <c r="C119" s="9">
-        <v>0</v>
-      </c>
-      <c r="D119" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75" hidden="1">
-      <c r="A120" s="13"/>
-      <c r="B120" s="12"/>
-      <c r="C120" s="9">
-        <v>0</v>
-      </c>
-      <c r="D120" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75" hidden="1">
-      <c r="A121" s="13"/>
-      <c r="B121" s="12"/>
-      <c r="C121" s="9">
-        <v>0</v>
-      </c>
-      <c r="D121" s="10">
-        <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75" hidden="1">
-      <c r="A122" s="13"/>
-      <c r="B122" s="12"/>
       <c r="C122" s="9">
         <v>0</v>
       </c>
@@ -6338,9 +6210,13 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75" hidden="1">
-      <c r="A123" s="13"/>
-      <c r="B123" s="12"/>
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
+      <c r="A123" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C123" s="9">
         <v>0</v>
       </c>
@@ -6348,9 +6224,13 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75" hidden="1">
-      <c r="A124" s="13"/>
-      <c r="B124" s="12"/>
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
+      <c r="A124" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C124" s="9">
         <v>0</v>
       </c>
@@ -6358,9 +6238,13 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75" hidden="1">
-      <c r="A125" s="13"/>
-      <c r="B125" s="12"/>
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
+      <c r="A125" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C125" s="9">
         <v>0</v>
       </c>
@@ -6368,9 +6252,9 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75" hidden="1">
-      <c r="A126" s="13"/>
-      <c r="B126" s="12"/>
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
       <c r="C126" s="9">
         <v>0</v>
       </c>
@@ -6378,8 +6262,8 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75" hidden="1">
-      <c r="A127" s="13"/>
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
+      <c r="A127" s="11"/>
       <c r="B127" s="12"/>
       <c r="C127" s="9">
         <v>0</v>
@@ -6388,8 +6272,8 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75" hidden="1">
-      <c r="A128" s="13"/>
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
+      <c r="A128" s="12"/>
       <c r="B128" s="12"/>
       <c r="C128" s="9">
         <v>0</v>
@@ -6398,8 +6282,8 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75" hidden="1">
-      <c r="A129" s="13"/>
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
+      <c r="A129" s="11"/>
       <c r="B129" s="12"/>
       <c r="C129" s="9">
         <v>0</v>
@@ -6408,8 +6292,8 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75" hidden="1">
-      <c r="A130" s="13"/>
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
+      <c r="A130" s="11"/>
       <c r="B130" s="12"/>
       <c r="C130" s="9">
         <v>0</v>
@@ -6418,8 +6302,8 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75" hidden="1">
-      <c r="A131" s="13"/>
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
+      <c r="A131" s="11"/>
       <c r="B131" s="12"/>
       <c r="C131" s="9">
         <v>0</v>
@@ -6428,8 +6312,8 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75" hidden="1">
-      <c r="A132" s="13"/>
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
+      <c r="A132" s="11"/>
       <c r="B132" s="12"/>
       <c r="C132" s="9">
         <v>0</v>
@@ -6438,8 +6322,8 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75" hidden="1">
-      <c r="A133" s="13"/>
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
+      <c r="A133" s="11"/>
       <c r="B133" s="12"/>
       <c r="C133" s="9">
         <v>0</v>
@@ -6448,7 +6332,7 @@
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
       <c r="A134" s="13"/>
       <c r="B134" s="12"/>
       <c r="C134" s="9">
@@ -6459,224 +6343,160 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
-      <c r="A135" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A135" s="13"/>
+      <c r="B135" s="12"/>
       <c r="C135" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D135" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
-      <c r="A136" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A136" s="13"/>
+      <c r="B136" s="12"/>
       <c r="C136" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D136" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
-      <c r="A137" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A137" s="13"/>
+      <c r="B137" s="12"/>
       <c r="C137" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D137" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
-      <c r="A138" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A138" s="13"/>
+      <c r="B138" s="12"/>
       <c r="C138" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D138" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
-      <c r="A139" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A139" s="13"/>
+      <c r="B139" s="12"/>
       <c r="C139" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D139" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
-      <c r="A140" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A140" s="13"/>
+      <c r="B140" s="12"/>
       <c r="C140" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D140" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
-      <c r="A141" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A141" s="13"/>
+      <c r="B141" s="12"/>
       <c r="C141" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D141" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
-      <c r="A142" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A142" s="13"/>
+      <c r="B142" s="12"/>
       <c r="C142" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D142" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
-      <c r="A143" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A143" s="13"/>
+      <c r="B143" s="12"/>
       <c r="C143" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D143" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
-      <c r="A144" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A144" s="13"/>
+      <c r="B144" s="12"/>
       <c r="C144" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D144" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
-      <c r="A145" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A145" s="13"/>
+      <c r="B145" s="12"/>
       <c r="C145" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D145" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
-      <c r="A146" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A146" s="13"/>
+      <c r="B146" s="12"/>
       <c r="C146" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D146" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
-      <c r="A147" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A147" s="13"/>
+      <c r="B147" s="12"/>
       <c r="C147" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D147" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
-      <c r="A148" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A148" s="13"/>
+      <c r="B148" s="12"/>
       <c r="C148" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D148" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
-      <c r="A149" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A149" s="13"/>
+      <c r="B149" s="12"/>
       <c r="C149" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D149" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
-      <c r="A150" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A150" s="13"/>
+      <c r="B150" s="12"/>
       <c r="C150" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D150" s="10">
         <f>REPT("⭐",Tableau24[[#This Row], [Niveau]])</f>
@@ -7394,7 +7214,7 @@
       <c r="B74" s="3"/>
       <c r="C74" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="15.6">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="15.65">
       <c r="A75" s="1"/>
       <c r="B75" s="3"/>
       <c r="C75" s="1"/>

</xml_diff>